<commit_message>
Thetis integration for tuning algorithm
Numerous small changes to make the algorithm interface to Thetis
</commit_message>
<xml_diff>
--- a/documentation/atu toroids.xlsx
+++ b/documentation/atu toroids.xlsx
@@ -5,14 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Loz\SkyDrive\documents\amateur radio\SDR\aries_ATU\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Loz\SkyDrive\documents\amateur radio\SDR\Aries-ATU\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="11385"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="11385" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="1st prototype" sheetId="1" r:id="rId1"/>
+    <sheet name="Revised" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="21">
   <si>
     <t>target inductance</t>
   </si>
@@ -60,12 +61,43 @@
   </si>
   <si>
     <t>T68-6</t>
+  </si>
+  <si>
+    <t>Capacitors, Inductors all reduced to accept limitation on Topband and have better resolution on the other bands</t>
+  </si>
+  <si>
+    <t>Toroid</t>
+  </si>
+  <si>
+    <t>Al</t>
+  </si>
+  <si>
+    <t>Achieved inductance uH</t>
+  </si>
+  <si>
+    <t>target inductance uH</t>
+  </si>
+  <si>
+    <t>T106-6</t>
+  </si>
+  <si>
+    <t>Calc Turns</t>
+  </si>
+  <si>
+    <t>Actual turns</t>
+  </si>
+  <si>
+    <t>Measured inductance uH</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -91,7 +123,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -114,18 +146,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -409,8 +460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,26 +471,26 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3" t="s">
+      <c r="E1" s="8"/>
+      <c r="F1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3" t="s">
+      <c r="G1" s="8"/>
+      <c r="H1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3" t="s">
+      <c r="I1" s="8"/>
+      <c r="J1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="3"/>
+      <c r="K1" s="8"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -733,10 +784,10 @@
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="3"/>
+      <c r="C15" s="8"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -857,4 +908,288 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1">
+        <f>VLOOKUP(B4,A$14:B$17,2,FALSE)</f>
+        <v>47</v>
+      </c>
+      <c r="D4" s="7">
+        <f>SQRT(A4*10000/C4)</f>
+        <v>2.062842492517587</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2</v>
+      </c>
+      <c r="F4" s="9">
+        <f>C4*E4*E4/10000</f>
+        <v>1.8800000000000001E-2</v>
+      </c>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" ref="C5:C11" si="0">VLOOKUP(B5,A$14:B$17,2,FALSE)</f>
+        <v>47</v>
+      </c>
+      <c r="D5" s="7">
+        <f t="shared" ref="D5:D11" si="1">SQRT(A5*10000/C5)</f>
+        <v>2.9172998299578912</v>
+      </c>
+      <c r="E5" s="1">
+        <v>3</v>
+      </c>
+      <c r="F5" s="6">
+        <f t="shared" ref="F5:F11" si="2">C5*E5*E5/10000</f>
+        <v>4.2299999999999997E-2</v>
+      </c>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D6" s="7">
+        <f t="shared" si="1"/>
+        <v>4.125684985035174</v>
+      </c>
+      <c r="E6" s="1">
+        <v>4</v>
+      </c>
+      <c r="F6" s="6">
+        <f t="shared" si="2"/>
+        <v>7.5200000000000003E-2</v>
+      </c>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>0.16</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D7" s="7">
+        <f t="shared" si="1"/>
+        <v>5.8345996599157823</v>
+      </c>
+      <c r="E7" s="1">
+        <v>6</v>
+      </c>
+      <c r="F7" s="6">
+        <f t="shared" si="2"/>
+        <v>0.16919999999999999</v>
+      </c>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>0.32</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D8" s="7">
+        <f t="shared" si="1"/>
+        <v>8.251369970070348</v>
+      </c>
+      <c r="E8" s="1">
+        <v>8</v>
+      </c>
+      <c r="F8" s="6">
+        <f t="shared" si="2"/>
+        <v>0.30080000000000001</v>
+      </c>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>0.64</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="D9" s="7">
+        <f t="shared" si="1"/>
+        <v>10.59625885652035</v>
+      </c>
+      <c r="E9" s="1">
+        <v>11</v>
+      </c>
+      <c r="F9" s="6">
+        <f t="shared" si="2"/>
+        <v>0.68969999999999998</v>
+      </c>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>1.28</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="D10" s="7">
+        <f t="shared" si="1"/>
+        <v>14.985372985307103</v>
+      </c>
+      <c r="E10" s="1">
+        <v>15</v>
+      </c>
+      <c r="F10" s="6">
+        <f t="shared" si="2"/>
+        <v>1.2825</v>
+      </c>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>2.56</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="D11" s="7">
+        <f t="shared" si="1"/>
+        <v>21.192517713040701</v>
+      </c>
+      <c r="E11" s="1">
+        <v>21</v>
+      </c>
+      <c r="F11" s="6">
+        <f t="shared" si="2"/>
+        <v>2.5137</v>
+      </c>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="1">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="1">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="1">
+        <v>116</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Rev 4 hardware; code changes to integrate better to thetis
</commit_message>
<xml_diff>
--- a/documentation/atu toroids.xlsx
+++ b/documentation/atu toroids.xlsx
@@ -1,31 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Loz\SkyDrive\documents\amateur radio\SDR\Aries-ATU\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3d529807eb1393ed/documents/amateur radio/SDR/Aries-ATU/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="83" documentId="11_27A611F330B71D75F616A5C824CEB28B18A90973" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{405B7E9A-E3EB-461E-8DE6-3AF0CF0D4767}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="11385" activeTab="1"/>
+    <workbookView xWindow="8340" yWindow="1770" windowWidth="17415" windowHeight="10695" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1st prototype" sheetId="1" r:id="rId1"/>
     <sheet name="Revised" sheetId="2" r:id="rId2"/>
+    <sheet name="prototype 2 revised again" sheetId="4" r:id="rId3"/>
+    <sheet name="prototype 2" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="50">
   <si>
     <t>target inductance</t>
   </si>
@@ -157,12 +169,30 @@
   </si>
   <si>
     <t>T94-6</t>
+  </si>
+  <si>
+    <t>try 2T 0.3" dia 0.15" length</t>
+  </si>
+  <si>
+    <t>combined value (pF)</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>try 3T 0.3" dia 0.2" length</t>
+  </si>
+  <si>
+    <t>non-E12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -536,10 +566,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A29" sqref="A29:C38"/>
     </sheetView>
   </sheetViews>
@@ -1119,7 +1149,7 @@
     <mergeCell ref="I1:J1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B27" r:id="rId1"/>
+    <hyperlink ref="B27" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId2"/>
@@ -1127,10 +1157,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A3:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1561,4 +1593,909 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E37B9C1-BEB8-4BEA-8473-F3FEC66AAF77}">
+  <dimension ref="A2:G33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <f t="shared" ref="A3:A8" si="0">A4/2</f>
+        <v>2.34375E-2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="1">
+        <f>VLOOKUP(B3,A$14:B$23,2,FALSE)</f>
+        <v>70</v>
+      </c>
+      <c r="D3" s="7">
+        <f>SQRT(A3*10000/C3)</f>
+        <v>1.8298126367784997</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="8">
+        <f>C3*E3*E3/10000</f>
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <f t="shared" si="0"/>
+        <v>4.6875E-2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="1">
+        <f t="shared" ref="C4:C10" si="1">VLOOKUP(B4,A$14:B$23,2,FALSE)</f>
+        <v>70</v>
+      </c>
+      <c r="D4" s="7">
+        <f t="shared" ref="D4:D10" si="2">SQRT(A4*10000/C4)</f>
+        <v>2.5877458475338284</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2</v>
+      </c>
+      <c r="F4" s="6">
+        <f t="shared" ref="F4:F10" si="3">C4*E4*E4/10000</f>
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <f t="shared" si="0"/>
+        <v>9.375E-2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="D5" s="7">
+        <f t="shared" si="2"/>
+        <v>3.6596252735569994</v>
+      </c>
+      <c r="E5" s="1">
+        <v>4</v>
+      </c>
+      <c r="F5" s="6">
+        <f t="shared" si="3"/>
+        <v>0.112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <f t="shared" si="0"/>
+        <v>0.1875</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="D6" s="7">
+        <f t="shared" si="2"/>
+        <v>5.1754916950676568</v>
+      </c>
+      <c r="E6" s="1">
+        <v>5</v>
+      </c>
+      <c r="F6" s="6">
+        <f t="shared" si="3"/>
+        <v>0.17499999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <f t="shared" si="0"/>
+        <v>0.375</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+      <c r="D7" s="7">
+        <f t="shared" si="2"/>
+        <v>6.6815310478106102</v>
+      </c>
+      <c r="E7" s="1">
+        <v>7</v>
+      </c>
+      <c r="F7" s="6">
+        <f t="shared" si="3"/>
+        <v>0.41160000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+      <c r="D8" s="7">
+        <f t="shared" si="2"/>
+        <v>9.4491118252306805</v>
+      </c>
+      <c r="E8" s="1">
+        <v>9</v>
+      </c>
+      <c r="F8" s="6">
+        <f t="shared" si="3"/>
+        <v>0.6804</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <f>A10/2</f>
+        <v>1.5</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+      <c r="D9" s="7">
+        <f t="shared" si="2"/>
+        <v>13.36306209562122</v>
+      </c>
+      <c r="E9" s="1">
+        <v>13</v>
+      </c>
+      <c r="F9" s="6">
+        <f t="shared" si="3"/>
+        <v>1.4196</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="1">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+      <c r="D10" s="7">
+        <f t="shared" si="2"/>
+        <v>18.898223650461361</v>
+      </c>
+      <c r="E10" s="1">
+        <v>19</v>
+      </c>
+      <c r="F10" s="6">
+        <f t="shared" si="3"/>
+        <v>3.0324</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="1">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="1">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="1">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="1">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="1">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="7">
+        <f t="shared" ref="B26:B31" si="4">B27/2</f>
+        <v>21.09375</v>
+      </c>
+      <c r="C26" s="1">
+        <v>20</v>
+      </c>
+      <c r="D26" s="1">
+        <f>C26/2</f>
+        <v>10</v>
+      </c>
+      <c r="E26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="7">
+        <f t="shared" si="4"/>
+        <v>42.1875</v>
+      </c>
+      <c r="C27" s="1">
+        <v>39</v>
+      </c>
+      <c r="D27" s="1">
+        <f>C27/2</f>
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="7">
+        <f t="shared" si="4"/>
+        <v>84.375</v>
+      </c>
+      <c r="C28" s="1">
+        <v>82</v>
+      </c>
+      <c r="D28" s="1">
+        <f t="shared" ref="D28:D33" si="5">C28/2</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="7">
+        <f t="shared" si="4"/>
+        <v>168.75</v>
+      </c>
+      <c r="C29" s="1">
+        <v>180</v>
+      </c>
+      <c r="D29" s="1">
+        <f t="shared" si="5"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="1">
+        <f t="shared" si="4"/>
+        <v>337.5</v>
+      </c>
+      <c r="C30" s="1">
+        <v>330</v>
+      </c>
+      <c r="D30" s="1">
+        <f t="shared" si="5"/>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="1">
+        <f t="shared" si="4"/>
+        <v>675</v>
+      </c>
+      <c r="C31" s="1">
+        <v>680</v>
+      </c>
+      <c r="D31" s="1">
+        <f t="shared" si="5"/>
+        <v>340</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="1">
+        <f>B33/2</f>
+        <v>1350</v>
+      </c>
+      <c r="C32" s="1">
+        <v>1300</v>
+      </c>
+      <c r="D32" s="1">
+        <f t="shared" si="5"/>
+        <v>650</v>
+      </c>
+      <c r="E32" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="1">
+        <v>2700</v>
+      </c>
+      <c r="C33" s="1">
+        <v>2700</v>
+      </c>
+      <c r="D33" s="1">
+        <f t="shared" si="5"/>
+        <v>1350</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A2:F33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="1">
+        <f>VLOOKUP(B3,A$14:B$23,2,FALSE)</f>
+        <v>70</v>
+      </c>
+      <c r="D3" s="7">
+        <f>SQRT(A3*10000/C3)</f>
+        <v>2.3904572186687871</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2</v>
+      </c>
+      <c r="F3" s="8">
+        <f>C3*E3*E3/10000</f>
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="1">
+        <f t="shared" ref="C4:C10" si="0">VLOOKUP(B4,A$14:B$23,2,FALSE)</f>
+        <v>70</v>
+      </c>
+      <c r="D4" s="7">
+        <f t="shared" ref="D4:D10" si="1">SQRT(A4*10000/C4)</f>
+        <v>3.3806170189140663</v>
+      </c>
+      <c r="E4" s="1">
+        <v>3</v>
+      </c>
+      <c r="F4" s="6">
+        <f t="shared" ref="F4:F10" si="2">C4*E4*E4/10000</f>
+        <v>6.3E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>0.18</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="D5" s="7">
+        <f t="shared" si="1"/>
+        <v>5.0709255283710997</v>
+      </c>
+      <c r="E5" s="1">
+        <v>5</v>
+      </c>
+      <c r="F5" s="6">
+        <f t="shared" si="2"/>
+        <v>0.17499999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>0.312</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" si="0"/>
+        <v>84</v>
+      </c>
+      <c r="D6" s="7">
+        <f t="shared" si="1"/>
+        <v>6.0944940022004408</v>
+      </c>
+      <c r="E6" s="1">
+        <v>6</v>
+      </c>
+      <c r="F6" s="6">
+        <f t="shared" si="2"/>
+        <v>0.3024</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" si="0"/>
+        <v>84</v>
+      </c>
+      <c r="D7" s="7">
+        <f t="shared" si="1"/>
+        <v>8.6258194917794278</v>
+      </c>
+      <c r="E7" s="1">
+        <v>8</v>
+      </c>
+      <c r="F7" s="6">
+        <f t="shared" si="2"/>
+        <v>0.53759999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>1.25</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" si="0"/>
+        <v>84</v>
+      </c>
+      <c r="D8" s="7">
+        <f t="shared" si="1"/>
+        <v>12.198750911856663</v>
+      </c>
+      <c r="E8" s="1">
+        <v>12</v>
+      </c>
+      <c r="F8" s="6">
+        <f t="shared" si="2"/>
+        <v>1.2096</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" si="0"/>
+        <v>84</v>
+      </c>
+      <c r="D9" s="7">
+        <f t="shared" si="1"/>
+        <v>17.251638983558856</v>
+      </c>
+      <c r="E9" s="1">
+        <v>17</v>
+      </c>
+      <c r="F9" s="6">
+        <f t="shared" si="2"/>
+        <v>2.4276</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="1">
+        <f t="shared" si="0"/>
+        <v>84</v>
+      </c>
+      <c r="D10" s="7">
+        <f t="shared" si="1"/>
+        <v>24.397501823713327</v>
+      </c>
+      <c r="E10" s="1">
+        <v>24</v>
+      </c>
+      <c r="F10" s="6">
+        <f t="shared" si="2"/>
+        <v>4.8384</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="1">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="1">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="1">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="1">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="1">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26">
+        <v>18</v>
+      </c>
+      <c r="C26">
+        <f>B26/2</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27">
+        <v>39</v>
+      </c>
+      <c r="C27">
+        <f>B27/2</f>
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28">
+        <v>82</v>
+      </c>
+      <c r="C28">
+        <f t="shared" ref="C28:C33" si="3">B28/2</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29">
+        <v>150</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="3"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30">
+        <v>330</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="3"/>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31">
+        <v>680</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="3"/>
+        <v>340</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32">
+        <v>1500</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="3"/>
+        <v>750</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33">
+        <v>3300</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="3"/>
+        <v>1650</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>